<commit_message>
ENH: Before constraint notes cleanup
</commit_message>
<xml_diff>
--- a/MISO/Constraint Analyses/Top Congestion Reports/Aug-24_RT.xlsx
+++ b/MISO/Constraint Analyses/Top Congestion Reports/Aug-24_RT.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roscommonanalytics-my.sharepoint.com/personal/lgraham_roscommonanalytics_com/Documents/Documents/Obsidian_Vault/MISO/Constraint Analyses/Top Congestion Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{028F3325-8580-4112-B1CE-2BB285DE3E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA60C57D-BE1D-4C5B-A1AE-C00DE7449D38}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{028F3325-8580-4112-B1CE-2BB285DE3E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40CFC462-3D48-45C2-A9D1-F9B3D8BA2C81}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="57495" yWindow="1140" windowWidth="29010" windowHeight="15780" activeTab="2" xr2:uid="{82DFB18D-5167-4FE6-877E-FE1C49D9267F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{82DFB18D-5167-4FE6-877E-FE1C49D9267F}"/>
   </bookViews>
   <sheets>
     <sheet name="Aug-24 RT Pk" sheetId="1" r:id="rId1"/>
     <sheet name="Aug-24 RT Off" sheetId="2" r:id="rId2"/>
-    <sheet name="Merged" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="127">
   <si>
     <t>cid</t>
   </si>
@@ -824,7 +823,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -2856,158 +2855,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABF1981-EE90-409C-9D9E-4E28C862DBC8}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:A27"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A27">
-    <sortCondition ref="A1:A27"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>